<commit_message>
[Jimmy] correcion de forma y modificacion de excel
</commit_message>
<xml_diff>
--- a/src/assets/anexos/Anexo_Líneas_de_Crédito_CO.xlsx
+++ b/src/assets/anexos/Anexo_Líneas_de_Crédito_CO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/grp-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3A432A-E0B2-4A94-B25D-7411856723E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017FA9D2-30F3-5449-B1D9-A39FE06270E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0A66393D-A8A2-41B7-BA89-706438AD97E1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21100" xr2:uid="{0A66393D-A8A2-41B7-BA89-706438AD97E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Preaprobar líneas-de-crédito_CO" sheetId="2" r:id="rId1"/>
@@ -169,12 +169,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -490,117 +492,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3486B149-EEC3-4166-B481-C5614AD92EBD}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" customWidth="1"/>
-    <col min="10" max="10" width="16.54296875" customWidth="1"/>
-    <col min="11" max="11" width="15.36328125" customWidth="1"/>
-    <col min="12" max="12" width="14.6328125" customWidth="1"/>
-    <col min="13" max="13" width="16.26953125" customWidth="1"/>
-    <col min="14" max="14" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="2" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44992</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>10000</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="I3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>